<commit_message>
fix excel logic and some bug
</commit_message>
<xml_diff>
--- a/src/assets/invoice_template.xlsx
+++ b/src/assets/invoice_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HYUNJU_RYU\dev\smart-invoice\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6378F7-BC98-406D-8090-F19F87BFB559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D284D80-D245-4B98-84B3-5B381BECC27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8EA528CF-440F-4A42-A7F1-3323D257DF6E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8EA528CF-440F-4A42-A7F1-3323D257DF6E}"/>
   </bookViews>
   <sheets>
     <sheet name="合計請求明細書鑑" sheetId="1" r:id="rId1"/>
@@ -200,12 +200,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
-    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="178" formatCode="@\ &quot;御中&quot;"/>
-    <numFmt numFmtId="179" formatCode="[$$-409]#,##0.00;[$$-409]#,##0.00"/>
-    <numFmt numFmtId="180" formatCode="[$$-409]#,##0.00;\-[$$-409]#,##0.00"/>
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="177" formatCode="@\ &quot;御中&quot;"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -443,7 +440,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -468,16 +465,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -527,21 +524,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -989,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0ABCB3-B6F7-4F94-8113-B7AB31039D1B}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1009,14 +991,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="Y1" s="8"/>
+      <c r="Y1" s="10"/>
     </row>
     <row r="2" spans="1:26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
     </row>
     <row r="3" spans="1:26" customFormat="1" ht="33" x14ac:dyDescent="0.4">
       <c r="B3" s="12" t="s">
@@ -1047,8 +1029,8 @@
     </row>
     <row r="4" spans="1:26" customFormat="1" x14ac:dyDescent="0.4"/>
     <row r="5" spans="1:26" customFormat="1" ht="25.5" x14ac:dyDescent="0.4">
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:26" customFormat="1" x14ac:dyDescent="0.4"/>
     <row r="7" spans="1:26" customFormat="1" x14ac:dyDescent="0.4">
@@ -1140,26 +1122,7 @@
       <c r="Y14"/>
       <c r="Z14"/>
     </row>
-    <row r="15" spans="1:26" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="29"/>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29"/>
-      <c r="V15" s="30"/>
-    </row>
+    <row r="15" spans="1:26" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="1:26" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="17" spans="2:25" customFormat="1" x14ac:dyDescent="0.4"/>
     <row r="18" spans="2:25" s="7" customFormat="1" x14ac:dyDescent="0.4">
@@ -1248,7 +1211,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="10">
     <mergeCell ref="B3:X3"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
@@ -1257,20 +1220,13 @@
     <mergeCell ref="F11:O11"/>
     <mergeCell ref="N14:Q14"/>
     <mergeCell ref="R14:V14"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="R15:V15"/>
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="J14:M14"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="76" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddHeader>&amp;L１２３&amp;R１２３</oddHeader>
-  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1279,7 +1235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F297D11-1763-43C8-A105-CD640106E044}">
   <dimension ref="A1:GS948"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
@@ -4178,26 +4134,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0bb9526b-221f-43e7-a9ca-c97ff66af0d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0d2ed01c-d650-4e80-8773-04905e47c66a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="문서" ma:contentTypeID="0x0101002E3E4D0DB1C0F54BA6D82DB94AE8FE98" ma:contentTypeVersion="13" ma:contentTypeDescription="새 문서를 만듭니다." ma:contentTypeScope="" ma:versionID="fab01170fb8523c0a68c17ffe87dbeac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0bb9526b-221f-43e7-a9ca-c97ff66af0d6" xmlns:ns3="0d2ed01c-d650-4e80-8773-04905e47c66a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e3ff519f69ba9bca7f4f4c769429d0af" ns2:_="" ns3:_="">
     <xsd:import namespace="0bb9526b-221f-43e7-a9ca-c97ff66af0d6"/>
@@ -4404,10 +4340,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0bb9526b-221f-43e7-a9ca-c97ff66af0d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0d2ed01c-d650-4e80-8773-04905e47c66a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2ED7F77-F12D-4F2A-B958-2CE47797289F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB955BD1-E483-4700-B456-2F6C6DC8311B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0bb9526b-221f-43e7-a9ca-c97ff66af0d6"/>
+    <ds:schemaRef ds:uri="0d2ed01c-d650-4e80-8773-04905e47c66a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4424,20 +4391,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB955BD1-E483-4700-B456-2F6C6DC8311B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2ED7F77-F12D-4F2A-B958-2CE47797289F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0bb9526b-221f-43e7-a9ca-c97ff66af0d6"/>
-    <ds:schemaRef ds:uri="0d2ed01c-d650-4e80-8773-04905e47c66a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>